<commit_message>
adding info about partial and semi partial correlations
</commit_message>
<xml_diff>
--- a/WJ scores.xlsx
+++ b/WJ scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elisabeth/Desktop/UMASS/BKonline data/BK-Online-Replication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1137853-BDD6-A942-B788-22BEB398D9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB656D0-5DAA-304C-A8AB-E94D61AC7E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16440" xr2:uid="{EFD6AE72-DBDA-6944-A8CF-ED58475E50DD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>bkp066</t>
+  </si>
+  <si>
+    <t>bkp028</t>
   </si>
 </sst>
 </file>
@@ -596,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7673370-AB5F-594B-AA52-9A9AB11468A5}">
-  <dimension ref="A1:B1002"/>
+  <dimension ref="A1:B1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -662,199 +665,199 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>51</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1">
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1">
-        <v>19</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1">
-        <v>61</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1">
-        <v>40</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1">
-        <v>72</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1">
-        <v>49</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1">
-        <v>69</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1">
         <v>47</v>
@@ -862,138 +865,138 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="1">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1">
-        <v>39</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1">
-        <v>24</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1">
-        <v>60</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="1">
         <v>43</v>
-      </c>
-      <c r="B45" s="1">
-        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" s="1">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" s="1">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" s="1">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" s="1">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1001,132 +1004,136 @@
         <v>47</v>
       </c>
       <c r="B50" s="1">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B51" s="1">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B52" s="1">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B53" s="1">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B54" s="1">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B55" s="1">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B56" s="1">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B57" s="2">
-        <v>74</v>
+        <v>63</v>
+      </c>
+      <c r="B57" s="1">
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B58" s="2">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B59" s="2">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B60" s="2">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B61" s="1">
-        <v>76</v>
+        <v>56</v>
+      </c>
+      <c r="B61" s="2">
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B62" s="1">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B63" s="1">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B64" s="1">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B66" s="1">
         <v>77</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
@@ -4871,6 +4878,10 @@
     <row r="1002" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1002" s="1"/>
       <c r="B1002" s="1"/>
+    </row>
+    <row r="1003" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating glms and adding new graphs
</commit_message>
<xml_diff>
--- a/WJ scores.xlsx
+++ b/WJ scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elisabeth/Desktop/UMASS/BKonline data/BK-Online-Replication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB656D0-5DAA-304C-A8AB-E94D61AC7E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85356A0-F6C8-374C-A3DB-109CBB1C7109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16440" xr2:uid="{EFD6AE72-DBDA-6944-A8CF-ED58475E50DD}"/>
+    <workbookView xWindow="2720" yWindow="500" windowWidth="28040" windowHeight="16440" xr2:uid="{EFD6AE72-DBDA-6944-A8CF-ED58475E50DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -152,9 +152,6 @@
     <t>bkp060</t>
   </si>
   <si>
-    <t>bkp061</t>
-  </si>
-  <si>
     <t>bkp062</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>bkp028</t>
+  </si>
+  <si>
+    <t>bkp121</t>
   </si>
 </sst>
 </file>
@@ -599,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7673370-AB5F-594B-AA52-9A9AB11468A5}">
-  <dimension ref="A1:B1003"/>
+  <dimension ref="A1:B1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,7 +612,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -665,7 +665,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="1">
         <v>68</v>
@@ -924,7 +924,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="1">
-        <v>24</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -932,7 +932,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="1">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -940,7 +940,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="1">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -948,23 +948,23 @@
         <v>41</v>
       </c>
       <c r="B43" s="1">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="B44" s="1">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="B45" s="1">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -972,7 +972,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="1">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -980,7 +980,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="1">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -988,7 +988,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="1">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -996,7 +996,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="1">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1004,136 +1004,132 @@
         <v>47</v>
       </c>
       <c r="B50" s="1">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B51" s="1">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B52" s="1">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B53" s="1">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B54" s="1">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B55" s="1">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B56" s="1">
-        <v>70</v>
+      <c r="B56" s="2">
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B57" s="1">
+        <v>53</v>
+      </c>
+      <c r="B57" s="2">
         <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B58" s="2">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B59" s="2">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B60" s="2">
-        <v>65</v>
+        <v>56</v>
+      </c>
+      <c r="B60" s="1">
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B61" s="2">
-        <v>73</v>
+        <v>57</v>
+      </c>
+      <c r="B61" s="1">
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B62" s="1">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B63" s="1">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B64" s="1">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B65" s="1">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B66" s="1">
-        <v>77</v>
-      </c>
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
@@ -4875,15 +4871,10 @@
       <c r="A1001" s="1"/>
       <c r="B1001" s="1"/>
     </row>
-    <row r="1002" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1002" s="1"/>
-      <c r="B1002" s="1"/>
-    </row>
-    <row r="1003" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1003" s="1"/>
-      <c r="B1003" s="1"/>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B1001">
+    <sortCondition ref="A2:A1001"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>